<commit_message>
Added message box and auto generates error log file to list all found errors.
</commit_message>
<xml_diff>
--- a/Data/bills_of_materials-tmp.xlsx
+++ b/Data/bills_of_materials-tmp.xlsx
@@ -2566,8 +2566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Status bar added. Error notifications improved.
</commit_message>
<xml_diff>
--- a/Data/bills_of_materials-tmp.xlsx
+++ b/Data/bills_of_materials-tmp.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://globalimi-my.sharepoint.com/personal/bryndell_torio_global-imi_com/Documents/Design/Training/bomgen/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bryndell.torio\Documents\bomgen\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="14_{257B2BC6-9D9F-4B6E-9F1C-76F7B88330CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A0F375C-1FAE-44D1-91CE-161B7B998C6D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{938665C5-1741-4F7A-949C-3A0290B9984B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2566,8 +2566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L168"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2915,7 +2915,7 @@
         <v>11</v>
       </c>
       <c r="B25">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C25" t="s">
         <v>59</v>
@@ -3443,7 +3443,7 @@
         <v>29</v>
       </c>
       <c r="B43">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C43" t="s">
         <v>126</v>

</xml_diff>